<commit_message>
added send email to admin and employee not submitted
</commit_message>
<xml_diff>
--- a/tests/timesheet.xlsx
+++ b/tests/timesheet.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,13 +421,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Sakana Rajam</v>
+        <v>Harin Vimal Bharathi.J</v>
       </c>
       <c r="C2" t="str">
-        <v>Praveen Kumar B</v>
+        <v>Yuvaraj Shanmugam</v>
       </c>
       <c r="D2" t="str">
-        <v>sakanar@techcedence.com</v>
+        <v>harinj@techcedence.com</v>
       </c>
     </row>
     <row r="3">
@@ -435,13 +435,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>Sarathraj K</v>
+        <v>Sri Manikandan K</v>
       </c>
       <c r="C3" t="str">
-        <v>Praveen Kumar B</v>
+        <v>Poorna chandran R</v>
       </c>
       <c r="D3" t="str">
-        <v>sarathrajk@techcedence.com</v>
+        <v>srimanikandank@techcedence.com</v>
       </c>
     </row>
     <row r="4">
@@ -449,18 +449,377 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>Raneesha P</v>
+        <v>Krishna Kumar P</v>
       </c>
       <c r="C4" t="str">
-        <v>Praveen Kumar B</v>
+        <v>Karthick N Super Admin</v>
       </c>
       <c r="D4" t="str">
-        <v>raneeshap@techcedence.com</v>
+        <v>krishnak@techcedence.com</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Harish S</v>
+      </c>
+      <c r="C5" t="str">
+        <v>harishs@techcedence.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Anjali Krishna</v>
+      </c>
+      <c r="C6" t="str">
+        <v>anjalik@techcedence.com</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Santhosh Kumar M</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Prathamesh Rajput</v>
+      </c>
+      <c r="D7" t="str">
+        <v>santhoshk@techcedence.com</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Anil Kumar P</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Srinivasan N</v>
+      </c>
+      <c r="D8" t="str">
+        <v>anilk@techcedence.com</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Manikandan R</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Krishna Kumar P</v>
+      </c>
+      <c r="D9" t="str">
+        <v>manikandanr@techcedence.com</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Alan Singh P</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Yugendran G</v>
+      </c>
+      <c r="D10" t="str">
+        <v>alans@techcedence.com</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Sathish Kumar</v>
+      </c>
+      <c r="C11" t="str">
+        <v>sathishk@techcedence.com</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Vivekkumar Perinbaraj</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Saibali Barooah</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Vivekkumarp@techcedence.com</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Dhinakaran VP</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Venkatesh A</v>
+      </c>
+      <c r="D13" t="str">
+        <v>dhinakaranv@techcedence.com</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Venkateshwaran C</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Venkateshwaranc@techcedence.com</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Niket Shah</v>
+      </c>
+      <c r="C15" t="str">
+        <v>nikets@techcedence.com</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Kathiravan P</v>
+      </c>
+      <c r="C16" t="str">
+        <v>Golda G</v>
+      </c>
+      <c r="D16" t="str">
+        <v>kathiravanp@techcedence.com</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Karthik Vinod</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Prathamesh Rajput</v>
+      </c>
+      <c r="D17" t="str">
+        <v>karthikv@techcedence.com</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Saibali Barooah</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Krishna Kumar P</v>
+      </c>
+      <c r="D18" t="str">
+        <v>saibalib@techcedence.com</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Yugendran G</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Venkatesh A</v>
+      </c>
+      <c r="D19" t="str">
+        <v>yugendrang@techcedence.com</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Jayanth Kandregula</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Venkatesh A</v>
+      </c>
+      <c r="D20" t="str">
+        <v>jayanthk@techcedence.com</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Gobi J</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Krishna Kumar P</v>
+      </c>
+      <c r="D21" t="str">
+        <v>gobij@techcedence.com</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Manoowranjith A J</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Saravana Kumar</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Manoowranjitha@techcedence.com</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Sabarish K</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Gowtham R</v>
+      </c>
+      <c r="D23" t="str">
+        <v>sabarishk@techcedence.com</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Saravana Kumar</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Venkatesh A</v>
+      </c>
+      <c r="D24" t="str">
+        <v>saravanak@techcedence.com</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Prathamesh Rajput</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Krishna Kumar P</v>
+      </c>
+      <c r="D25" t="str">
+        <v>prathameshr@techcedence.com</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>25</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Gowrishankar.G</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Prathamesh Rajput</v>
+      </c>
+      <c r="D26" t="str">
+        <v>GowrishankarG@techcedence.com</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>26</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Venkat BCG</v>
+      </c>
+      <c r="C27" t="str">
+        <v>venkat@barcodegulf.net</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>27</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Mehdi S</v>
+      </c>
+      <c r="C28" t="str">
+        <v>mehdis@techcedence.com</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>28</v>
+      </c>
+      <c r="B29" t="str">
+        <v>dina001</v>
+      </c>
+      <c r="C29" t="str">
+        <v>dhinakaranv+1@techcedence.com</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>29</v>
+      </c>
+      <c r="B30" t="str">
+        <v>admin@techcedence.com</v>
+      </c>
+      <c r="C30" t="str">
+        <v>admin@techcedence.com</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>30</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Medi</v>
+      </c>
+      <c r="C31" t="str">
+        <v>mehdi.s@geevida.com</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>31</v>
+      </c>
+      <c r="B32" t="str">
+        <v>US Cricket Store</v>
+      </c>
+      <c r="C32" t="str">
+        <v>uscricstore@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>